<commit_message>
More additions and cleanings.
</commit_message>
<xml_diff>
--- a/releases.xlsx
+++ b/releases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADEBA5-79FE-4302-8BCD-405CA5E95F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4676F703-8CC0-44EC-B101-A327A4DA36E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$58</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="101">
   <si>
     <t>title</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>magyarzeldak.hu</t>
+  </si>
+  <si>
+    <t>videókat szét kell vágni, 50 mega felett van</t>
+  </si>
+  <si>
+    <t>Celeste Classic GBA</t>
+  </si>
+  <si>
+    <t>costlyclick</t>
   </si>
 </sst>
 </file>
@@ -705,13 +714,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I60" sqref="I55:I60"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,9 +1397,27 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>71</v>
@@ -1615,7 +1642,7 @@
         <v>83</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>76</v>
@@ -1675,6 +1702,9 @@
       <c r="H54" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="I54" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -1755,8 +1785,34 @@
         <v>71</v>
       </c>
     </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H58" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E48">
     <sortCondition ref="A2:A48"/>
   </sortState>

</xml_diff>

<commit_message>
Further cleanup and recheck
</commit_message>
<xml_diff>
--- a/releases.xlsx
+++ b/releases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4676F703-8CC0-44EC-B101-A327A4DA36E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03360E22-5CEA-46E6-BA3A-AEF94290C83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$58</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="107">
   <si>
     <t>title</t>
   </si>
@@ -211,9 +222,6 @@
     <t>latest change</t>
   </si>
   <si>
-    <t>releasenotes added, and also a screenshot iwth fil download url.</t>
-  </si>
-  <si>
     <t>Not yet.</t>
   </si>
   <si>
@@ -235,9 +243,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>added releasenotes</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -250,15 +255,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>added release notes</t>
-  </si>
-  <si>
     <t>need to have one.</t>
   </si>
   <si>
-    <t>added</t>
-  </si>
-  <si>
     <t>Retrobattle</t>
   </si>
   <si>
@@ -286,9 +285,6 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>extrac to subdirectory</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -326,6 +322,39 @@
   </si>
   <si>
     <t>costlyclick</t>
+  </si>
+  <si>
+    <t>gbatemp links are ok</t>
+  </si>
+  <si>
+    <t>új fajlok, shareware kell minimum, de tegyük mellé a fullt, ha van elérhető</t>
+  </si>
+  <si>
+    <t>eltünt a netről, törlés? Megnézni otthon mentésben</t>
+  </si>
+  <si>
+    <t>releasenotes</t>
+  </si>
+  <si>
+    <t>new entry added</t>
+  </si>
+  <si>
+    <t>extract target modified to a subdirectory</t>
+  </si>
+  <si>
+    <t>DLQRcode and releasenotes</t>
+  </si>
+  <si>
+    <t>hax0kartik</t>
+  </si>
+  <si>
+    <t>drive backup</t>
+  </si>
+  <si>
+    <t>gamedata.zip</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
@@ -407,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,6 +460,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -714,13 +746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:B40"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +768,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,123 +788,141 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="H6" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -884,27 +934,36 @@
         <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="H10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -912,10 +971,10 @@
         <v>52</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -923,10 +982,10 @@
         <v>54</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -934,18 +993,18 @@
         <v>50</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -953,25 +1012,25 @@
         <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -979,33 +1038,36 @@
         <v>58</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1013,25 +1075,28 @@
         <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1039,36 +1104,39 @@
         <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1076,10 +1144,10 @@
         <v>49</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1087,25 +1155,28 @@
         <v>58</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
@@ -1113,77 +1184,83 @@
         <v>58</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -1191,85 +1268,94 @@
         <v>58</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1277,44 +1363,47 @@
         <v>53</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1322,10 +1411,10 @@
         <v>52</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
@@ -1333,150 +1422,174 @@
         <v>58</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="B38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="H38" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
@@ -1484,33 +1597,36 @@
         <v>58</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -1518,10 +1634,10 @@
         <v>54</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>38</v>
       </c>
@@ -1529,286 +1645,316 @@
         <v>58</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>56</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J49" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J50" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="C52" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="J52" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="C55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I55" s="8"/>
+      <c r="J55" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G52" s="2" t="s">
+      <c r="C56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I55" s="8"/>
-    </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>80</v>
+      <c r="J58" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More cleanup and addition
</commit_message>
<xml_diff>
--- a/releases.xlsx
+++ b/releases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9AB03-8F96-4D1B-A0E5-11C01EF55143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BD3F40-B0E8-427B-A4E6-216E29931AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="192">
   <si>
     <t>title</t>
   </si>
@@ -585,6 +585,33 @@
   </si>
   <si>
     <t>3DiceRoll</t>
+  </si>
+  <si>
+    <t>JFBlood</t>
+  </si>
+  <si>
+    <t>Fallout 1 CE</t>
+  </si>
+  <si>
+    <t>Fallout 2 CE</t>
+  </si>
+  <si>
+    <t>https://github.com/MrHuu/dethrace-3ds</t>
+  </si>
+  <si>
+    <t>3 freeware 1 full files</t>
+  </si>
+  <si>
+    <t>Dethrace</t>
+  </si>
+  <si>
+    <t>EasyRPGPlayer</t>
+  </si>
+  <si>
+    <t>EasyRPG</t>
+  </si>
+  <si>
+    <t>needs morexperiment, top free games to download, some release notes abot using other games</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1065,10 @@
   <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2833,7 +2860,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>178</v>
       </c>
@@ -2859,7 +2886,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>177</v>
       </c>
@@ -2885,7 +2912,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="15" t="s">
         <v>182</v>
       </c>
@@ -2911,7 +2938,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="15" t="s">
         <v>180</v>
       </c>
@@ -2937,18 +2964,134 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I72" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I73" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>115</v>
       </c>
@@ -2962,7 +3105,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>117</v>
       </c>
@@ -2976,7 +3119,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A79" s="12" t="s">
         <v>118</v>
       </c>
@@ -2990,7 +3133,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Adding titles to todo list
</commit_message>
<xml_diff>
--- a/releases.xlsx
+++ b/releases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0AFDC-7456-41EF-B2D7-B733F18F289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB0BFD8-DAEC-467A-BADB-39AF2E8C02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="271">
   <si>
     <t>title</t>
   </si>
@@ -721,12 +721,180 @@
   <si>
     <t>sikertelen, de elérhető</t>
   </si>
+  <si>
+    <t>Yet Another Flappy Bird. With Vertical Orientation</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/374</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/372</t>
+  </si>
+  <si>
+    <t>Terri-Fried</t>
+  </si>
+  <si>
+    <t>Wordle 3DS ASCII Game</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/361</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/358</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/357</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>CIA Installer</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/355</t>
+  </si>
+  <si>
+    <t>3dXMMP</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/348</t>
+  </si>
+  <si>
+    <t>3DSoundboard</t>
+  </si>
+  <si>
+    <t>Slime Of Schrödinger</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/347</t>
+  </si>
+  <si>
+    <t>SuDokuL </t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/345</t>
+  </si>
+  <si>
+    <t>Cube Adventures</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/332</t>
+  </si>
+  <si>
+    <t>újranézni</t>
+  </si>
+  <si>
+    <t>Multi-PokemonFramework+</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/326</t>
+  </si>
+  <si>
+    <t>Bandolero 3Ds</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/324</t>
+  </si>
+  <si>
+    <t>Level256 Network Installer</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/319</t>
+  </si>
+  <si>
+    <t>3DSx Play Coin Setter Mod</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/318</t>
+  </si>
+  <si>
+    <t>Dead Pixel Checker</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/317</t>
+  </si>
+  <si>
+    <t>Anarch - Suckless FPS game</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/316</t>
+  </si>
+  <si>
+    <t>Touch Keys</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/312</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/307</t>
+  </si>
+  <si>
+    <t>budgieSSH (An SSH client for the 3DS)</t>
+  </si>
+  <si>
+    <t>Terminal interface clicker game</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/306</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/304</t>
+  </si>
+  <si>
+    <t>Donut.c </t>
+  </si>
+  <si>
+    <t>RollTheDice-3DS</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/293</t>
+  </si>
+  <si>
+    <t>Space Invaders Clone</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/289</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/288</t>
+  </si>
+  <si>
+    <t>Notebook3DS</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/287</t>
+  </si>
+  <si>
+    <t>3DS Collab Doodle App</t>
+  </si>
+  <si>
+    <t>3DiceRoll/3DiceRoller</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/274</t>
+  </si>
+  <si>
+    <t>1.1.0 !!!!</t>
+  </si>
+  <si>
+    <t>3DS Button Tester</t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/273</t>
+  </si>
+  <si>
+    <t>BlargSPC 3ds </t>
+  </si>
+  <si>
+    <t>https://github.com/Universal-Team/db/issues/268</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,6 +978,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="13">
@@ -899,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -977,6 +1152,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -1264,31 +1440,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A85" sqref="A85"/>
+      <selection pane="bottomRight" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" style="1"/>
-    <col min="11" max="11" width="35.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="27.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="1"/>
+    <col min="11" max="11" width="35.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1499,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -1361,7 +1537,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>160</v>
       </c>
@@ -1399,7 +1575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -1437,7 +1613,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1475,7 +1651,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1513,7 +1689,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>150</v>
       </c>
@@ -1551,7 +1727,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>158</v>
       </c>
@@ -1589,7 +1765,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>157</v>
       </c>
@@ -1627,7 +1803,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1841,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -1703,7 +1879,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>154</v>
       </c>
@@ -1741,7 +1917,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>200</v>
       </c>
@@ -1779,7 +1955,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1817,7 +1993,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1855,7 +2031,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1893,7 +2069,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1932,7 +2108,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>139</v>
       </c>
@@ -1971,7 +2147,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>140</v>
       </c>
@@ -2009,7 +2185,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>167</v>
       </c>
@@ -2047,7 +2223,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>162</v>
       </c>
@@ -2085,7 +2261,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>163</v>
       </c>
@@ -2123,7 +2299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>156</v>
       </c>
@@ -2161,7 +2337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -2199,7 +2375,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>173</v>
       </c>
@@ -2278,7 +2454,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -2316,7 +2492,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -2354,7 +2530,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>161</v>
       </c>
@@ -2392,7 +2568,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2430,7 +2606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -2468,7 +2644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -2506,7 +2682,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2545,7 +2721,7 @@
       </c>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -2582,7 +2758,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
@@ -2620,7 +2796,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
@@ -2658,7 +2834,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -2696,7 +2872,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>32</v>
       </c>
@@ -2734,7 +2910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -2772,7 +2948,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -2848,7 +3024,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -2886,7 +3062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>18</v>
       </c>
@@ -2924,7 +3100,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>7</v>
       </c>
@@ -2945,7 +3121,7 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>29</v>
       </c>
@@ -2983,7 +3159,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
@@ -3021,7 +3197,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>1</v>
       </c>
@@ -3097,7 +3273,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -3135,7 +3311,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3349,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -3211,7 +3387,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>30</v>
       </c>
@@ -3249,7 +3425,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>23</v>
       </c>
@@ -3287,7 +3463,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
@@ -3325,7 +3501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>26</v>
       </c>
@@ -3363,7 +3539,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>27</v>
       </c>
@@ -3401,7 +3577,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
@@ -3439,7 +3615,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -3477,7 +3653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -3515,7 +3691,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>67</v>
       </c>
@@ -3553,7 +3729,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -3591,7 +3767,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>99</v>
       </c>
@@ -3611,7 +3787,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>16</v>
       </c>
@@ -3652,7 +3828,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>180</v>
       </c>
@@ -3690,7 +3866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>17</v>
       </c>
@@ -3726,7 +3902,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>21</v>
       </c>
@@ -3764,7 +3940,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>31</v>
       </c>
@@ -3800,7 +3976,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>202</v>
       </c>
@@ -3836,12 +4012,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>144</v>
       </c>
@@ -3859,8 +4035,11 @@
       <c r="K72" s="10" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N72" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>141</v>
       </c>
@@ -3878,13 +4057,16 @@
       <c r="K73" s="10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N73" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>104</v>
       </c>
@@ -3898,7 +4080,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>133</v>
       </c>
@@ -3915,7 +4097,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>149</v>
       </c>
@@ -3923,7 +4105,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
@@ -3937,7 +4119,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>166</v>
       </c>
@@ -3954,7 +4136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -3968,7 +4150,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
         <v>105</v>
       </c>
@@ -3982,7 +4164,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>125</v>
       </c>
@@ -3996,16 +4178,16 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>119</v>
       </c>
@@ -4017,6 +4199,225 @@
       </c>
       <c r="H89" s="1" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A104" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A106" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A107" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A108" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A110" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A111" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A112" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A118" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -4026,8 +4427,9 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="M34" r:id="rId1" xr:uid="{A3E5B044-85D1-468A-A613-8725F60707A8}"/>
+    <hyperlink ref="A96" r:id="rId2" display="https://github.com/Universal-Team/db/issues/357" xr:uid="{70329A6B-E196-48D4-8022-8F632C2E1858}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New additions and corrections
</commit_message>
<xml_diff>
--- a/releases.xlsx
+++ b/releases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB0BFD8-DAEC-467A-BADB-39AF2E8C02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176B52D-C1AD-40FD-B8C6-1F29F4EEA7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11268" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="274">
   <si>
     <t>title</t>
   </si>
@@ -888,6 +889,15 @@
   </si>
   <si>
     <t>https://github.com/Universal-Team/db/issues/268</t>
+  </si>
+  <si>
+    <t>van</t>
+  </si>
+  <si>
+    <t>konvertálni</t>
+  </si>
+  <si>
+    <t>nincs, készíteni</t>
   </si>
 </sst>
 </file>
@@ -1443,28 +1453,28 @@
   <dimension ref="A1:N118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A118" sqref="A118"/>
+      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.28515625" style="1"/>
-    <col min="11" max="11" width="35.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.33203125" style="1"/>
+    <col min="11" max="11" width="35.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1509,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -1537,7 +1547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>160</v>
       </c>
@@ -1575,7 +1585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -1613,7 +1623,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1689,7 +1699,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>150</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>158</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>157</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1841,7 +1851,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -1879,7 +1889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>154</v>
       </c>
@@ -1917,7 +1927,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>200</v>
       </c>
@@ -1955,7 +1965,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2031,7 +2041,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2118,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>139</v>
       </c>
@@ -2147,7 +2157,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>140</v>
       </c>
@@ -2185,7 +2195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>167</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>162</v>
       </c>
@@ -2261,7 +2271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>163</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>156</v>
       </c>
@@ -2337,7 +2347,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -2375,7 +2385,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2413,7 +2423,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>173</v>
       </c>
@@ -2454,7 +2464,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -2492,7 +2502,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -2530,7 +2540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>161</v>
       </c>
@@ -2568,7 +2578,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2606,7 +2616,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -2644,7 +2654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -2682,7 +2692,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2721,7 +2731,7 @@
       </c>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -2758,7 +2768,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
@@ -2796,7 +2806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
@@ -2834,7 +2844,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>32</v>
       </c>
@@ -2910,7 +2920,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -2948,7 +2958,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>8</v>
       </c>
@@ -2986,7 +2996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -3024,7 +3034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -3062,7 +3072,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>18</v>
       </c>
@@ -3100,7 +3110,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>7</v>
       </c>
@@ -3121,7 +3131,7 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>29</v>
       </c>
@@ -3159,7 +3169,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
@@ -3197,7 +3207,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -3235,7 +3245,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>1</v>
       </c>
@@ -3273,7 +3283,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -3311,7 +3321,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
@@ -3349,7 +3359,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -3387,7 +3397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>30</v>
       </c>
@@ -3425,7 +3435,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
         <v>23</v>
       </c>
@@ -3463,7 +3473,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
@@ -3501,7 +3511,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>26</v>
       </c>
@@ -3539,7 +3549,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>27</v>
       </c>
@@ -3577,7 +3587,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
@@ -3615,7 +3625,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -3653,7 +3663,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -3691,7 +3701,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>67</v>
       </c>
@@ -3729,7 +3739,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -3767,7 +3777,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>99</v>
       </c>
@@ -3787,7 +3797,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>16</v>
       </c>
@@ -3828,7 +3838,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>180</v>
       </c>
@@ -3866,7 +3876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>17</v>
       </c>
@@ -3902,7 +3912,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>21</v>
       </c>
@@ -3940,7 +3950,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>31</v>
       </c>
@@ -3976,7 +3986,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>202</v>
       </c>
@@ -4012,12 +4022,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>144</v>
       </c>
@@ -4039,7 +4049,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>141</v>
       </c>
@@ -4061,12 +4071,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>104</v>
       </c>
@@ -4080,7 +4090,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>133</v>
       </c>
@@ -4097,7 +4107,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>149</v>
       </c>
@@ -4105,7 +4115,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
@@ -4119,7 +4129,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>166</v>
       </c>
@@ -4136,7 +4146,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -4150,7 +4160,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A84" s="9" t="s">
         <v>105</v>
       </c>
@@ -4164,7 +4174,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>125</v>
       </c>
@@ -4178,16 +4188,16 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>119</v>
       </c>
@@ -4201,15 +4211,21 @@
         <v>138</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I92" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>218</v>
       </c>
@@ -4217,15 +4233,21 @@
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I94" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>223</v>
       </c>
@@ -4233,7 +4255,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>224</v>
       </c>
@@ -4241,7 +4263,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>226</v>
       </c>
@@ -4249,7 +4271,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>228</v>
       </c>
@@ -4257,7 +4279,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>229</v>
       </c>
@@ -4265,7 +4287,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>231</v>
       </c>
@@ -4273,7 +4295,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A101" s="27" t="s">
         <v>233</v>
       </c>
@@ -4281,7 +4303,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A102" s="27" t="s">
         <v>236</v>
       </c>
@@ -4289,7 +4311,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A103" s="27" t="s">
         <v>238</v>
       </c>
@@ -4297,7 +4319,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A104" s="27" t="s">
         <v>240</v>
       </c>
@@ -4305,7 +4327,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A105" s="27" t="s">
         <v>242</v>
       </c>
@@ -4313,7 +4335,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A106" s="27" t="s">
         <v>244</v>
       </c>
@@ -4321,7 +4343,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A107" s="27" t="s">
         <v>246</v>
       </c>
@@ -4329,7 +4351,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A108" s="27" t="s">
         <v>248</v>
       </c>
@@ -4337,7 +4359,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A109" s="27" t="s">
         <v>251</v>
       </c>
@@ -4345,7 +4367,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A110" s="27" t="s">
         <v>252</v>
       </c>
@@ -4353,7 +4375,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A111" s="27" t="s">
         <v>255</v>
       </c>
@@ -4361,7 +4383,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A112" s="27" t="s">
         <v>256</v>
       </c>
@@ -4369,7 +4391,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A113" s="27" t="s">
         <v>258</v>
       </c>
@@ -4377,7 +4399,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A114" s="27" t="s">
         <v>261</v>
       </c>
@@ -4385,7 +4407,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A115" s="27" t="s">
         <v>263</v>
       </c>
@@ -4393,7 +4415,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A116" s="27" t="s">
         <v>264</v>
       </c>
@@ -4404,7 +4426,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A117" s="27" t="s">
         <v>267</v>
       </c>
@@ -4412,7 +4434,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A118" s="27" t="s">
         <v>269</v>
       </c>

</xml_diff>